<commit_message>
Change xlsxwriter to rust_xlsxwriter
</commit_message>
<xml_diff>
--- a/export/archivo.xlsx
+++ b/export/archivo.xlsx
@@ -97,12 +97,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF008000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -119,7 +125,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>

</xml_diff>

<commit_message>
Add dashboard logic and fix input type on sales view
</commit_message>
<xml_diff>
--- a/export/archivo.xlsx
+++ b/export/archivo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>ID Venta</t>
   </si>
@@ -34,6 +34,21 @@
     <t>ID Vendedor</t>
   </si>
   <si>
+    <t>XYZ-456</t>
+  </si>
+  <si>
+    <t>2024-10-29</t>
+  </si>
+  <si>
+    <t>HOW-349</t>
+  </si>
+  <si>
+    <t>ABC003</t>
+  </si>
+  <si>
+    <t>2022-04-01</t>
+  </si>
+  <si>
     <t>ABC011</t>
   </si>
   <si>
@@ -62,18 +77,6 @@
   </si>
   <si>
     <t>2023-08-30</t>
-  </si>
-  <si>
-    <t>ABC003</t>
-  </si>
-  <si>
-    <t>2022-04-01</t>
-  </si>
-  <si>
-    <t>OPQ-345</t>
-  </si>
-  <si>
-    <t>2024-11-23</t>
   </si>
 </sst>
 </file>
@@ -420,7 +423,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -448,7 +451,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -457,10 +460,10 @@
         <v>7</v>
       </c>
       <c r="D2">
-        <v>27999.99</v>
+        <v>7835</v>
       </c>
       <c r="E2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F2">
         <v>2</v>
@@ -468,16 +471,16 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D3">
-        <v>23999</v>
+        <v>7835</v>
       </c>
       <c r="E3">
         <v>3</v>
@@ -488,39 +491,39 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
       <c r="D4">
-        <v>49999.990000000005</v>
+        <v>19999.75</v>
       </c>
       <c r="E4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F4">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
       <c r="D5">
-        <v>47999</v>
+        <v>27999.99</v>
       </c>
       <c r="E5">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F5">
         <v>2</v>
@@ -528,61 +531,81 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
       <c r="D6">
-        <v>54999</v>
+        <v>23999</v>
       </c>
       <c r="E6">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
         <v>16</v>
       </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
       <c r="D7">
-        <v>2500.6400000000003</v>
+        <v>49999.990000000005</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
         <v>18</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8">
+        <v>47999</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
         <v>19</v>
       </c>
-      <c r="D8">
-        <v>29700</v>
-      </c>
-      <c r="E8">
-        <v>9</v>
-      </c>
-      <c r="F8">
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9">
+        <v>54999</v>
+      </c>
+      <c r="E9">
+        <v>6</v>
+      </c>
+      <c r="F9">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add export_vehicles service to main.rs
</commit_message>
<xml_diff>
--- a/export/archivo.xlsx
+++ b/export/archivo.xlsx
@@ -14,69 +14,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
-  <si>
-    <t>ID Venta</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+  <si>
+    <t>Nro chasis</t>
   </si>
   <si>
     <t>Matrícula</t>
   </si>
   <si>
-    <t>Fecha Venta</t>
-  </si>
-  <si>
-    <t>Precio Venta</t>
-  </si>
-  <si>
-    <t>ID Cliente</t>
-  </si>
-  <si>
-    <t>ID Vendedor</t>
-  </si>
-  <si>
-    <t>XYZ-456</t>
-  </si>
-  <si>
-    <t>2024-10-29</t>
-  </si>
-  <si>
-    <t>HOW-349</t>
-  </si>
-  <si>
-    <t>ABC003</t>
-  </si>
-  <si>
-    <t>2022-04-01</t>
-  </si>
-  <si>
-    <t>ABC011</t>
-  </si>
-  <si>
-    <t>2023-04-10</t>
-  </si>
-  <si>
-    <t>ABC015</t>
-  </si>
-  <si>
-    <t>2023-05-15</t>
-  </si>
-  <si>
-    <t>ABC019</t>
-  </si>
-  <si>
-    <t>2023-06-20</t>
-  </si>
-  <si>
-    <t>ABC023</t>
-  </si>
-  <si>
-    <t>2023-07-25</t>
-  </si>
-  <si>
-    <t>ABC027</t>
-  </si>
-  <si>
-    <t>2023-08-30</t>
+    <t>Modelo</t>
+  </si>
+  <si>
+    <t>Marca</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>anio</t>
+  </si>
+  <si>
+    <t>fecha_compra</t>
+  </si>
+  <si>
+    <t>precio_compra</t>
+  </si>
+  <si>
+    <t>estado</t>
+  </si>
+  <si>
+    <t>marcelo</t>
+  </si>
+  <si>
+    <t>memito</t>
+  </si>
+  <si>
+    <t>marcelito</t>
+  </si>
+  <si>
+    <t>2024-11-07</t>
+  </si>
+  <si>
+    <t>DISPONIBLE</t>
   </si>
 </sst>
 </file>
@@ -423,13 +402,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -448,165 +427,43 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2">
-        <v>1</v>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2">
-        <v>7835</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
       </c>
       <c r="F2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3">
-        <v>7835</v>
-      </c>
-      <c r="E3">
-        <v>3</v>
-      </c>
-      <c r="F3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4">
-        <v>19999.75</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
+        <v>2005</v>
+      </c>
+      <c r="G2" t="s">
         <v>12</v>
       </c>
-      <c r="D5">
-        <v>27999.99</v>
-      </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
-      <c r="F5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
         <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6">
-        <v>23999</v>
-      </c>
-      <c r="E6">
-        <v>3</v>
-      </c>
-      <c r="F6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7">
-        <v>49999.990000000005</v>
-      </c>
-      <c r="E7">
-        <v>4</v>
-      </c>
-      <c r="F7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8">
-        <v>47999</v>
-      </c>
-      <c r="E8">
-        <v>5</v>
-      </c>
-      <c r="F8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9">
-        <v>54999</v>
-      </c>
-      <c r="E9">
-        <v>6</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add flex direction column to dashboard charts card
</commit_message>
<xml_diff>
--- a/export/archivo.xlsx
+++ b/export/archivo.xlsx
@@ -14,48 +14,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
-  <si>
-    <t>Nro chasis</t>
-  </si>
-  <si>
-    <t>Matrícula</t>
-  </si>
-  <si>
-    <t>Modelo</t>
-  </si>
-  <si>
-    <t>Marca</t>
-  </si>
-  <si>
-    <t>color</t>
-  </si>
-  <si>
-    <t>anio</t>
-  </si>
-  <si>
-    <t>fecha_compra</t>
-  </si>
-  <si>
-    <t>precio_compra</t>
-  </si>
-  <si>
-    <t>estado</t>
-  </si>
-  <si>
-    <t>marcelo</t>
-  </si>
-  <si>
-    <t>memito</t>
-  </si>
-  <si>
-    <t>marcelito</t>
-  </si>
-  <si>
-    <t>2024-11-07</t>
-  </si>
-  <si>
-    <t>DISPONIBLE</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>id_cliente</t>
+  </si>
+  <si>
+    <t>nombre</t>
+  </si>
+  <si>
+    <t>apellido</t>
+  </si>
+  <si>
+    <t>cedula</t>
+  </si>
+  <si>
+    <t>Andres</t>
+  </si>
+  <si>
+    <t>guido</t>
+  </si>
+  <si>
+    <t>123</t>
   </si>
 </sst>
 </file>
@@ -402,13 +381,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -421,49 +400,19 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="D2" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2">
-        <v>2005</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>